<commit_message>
tooltip mapping xlsx for atom and gas framework
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -5,15 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92129\IdeaProjects\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B595F3C6-CB16-45A4-9A94-9BF24DD6B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C263E5-B27E-4A4C-98AA-D1244248D238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="2430" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Tooltip Mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -625,22 +626,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="6" customWidth="1"/>
-    <col min="4" max="4" width="35.08984375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="6" customWidth="1"/>
     <col min="6" max="12" width="15" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="6"/>
+    <col min="13" max="16384" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -706,7 +707,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -734,7 +735,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -762,7 +763,7 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -790,7 +791,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -818,7 +819,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -846,33 +847,47 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E145" s="8"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E146" s="8"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E147" s="8"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E148" s="8"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E170" s="8"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E171" s="8"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E172" s="8"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E173" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8998252D-8934-4923-BAE2-E6D038E56598}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -927,31 +942,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
-      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
-      <Description>JFHTZT72FDVU-254938863-279</Description>
-    </_dlc_DocIdUrl>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
-    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100135AEE51B13C7A4784C7A6FB658DD0E0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2ccf66da846160ccad12796df698db1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa7e5010-1311-4096-a344-326d1919664c" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="255ceb00-0504-4451-971c-89cf8ee3ad27" xmlns:ns5="953edb04-63dd-49ba-ad7b-e9d17e0e7f06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd9e9067e801230649229059a2f6238c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="fa7e5010-1311-4096-a344-326d1919664c"/>
@@ -1197,6 +1187,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
+      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
+      <Description>JFHTZT72FDVU-254938863-279</Description>
+    </_dlc_DocIdUrl>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
+    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E0ED53-E837-41F7-A9C9-5E67E49390EA}">
   <ds:schemaRefs>
@@ -1206,9 +1221,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1233,22 +1261,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change backend data structure
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D0B744-8F11-42F3-ABFA-2D188AEF2B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C6B73-60C3-4A92-A623-936547AB6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>Custom NuclearAndGasNonEligibleComponent</t>
+  </si>
+  <si>
+    <t>Referenced Reports</t>
+  </si>
+  <si>
+    <t>Please upload all relevant reports for this dataset in the PDF format.</t>
+  </si>
+  <si>
+    <t>Report Preupload</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
 </sst>
 </file>
@@ -389,15 +401,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -459,6 +462,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -466,7 +480,9 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -518,19 +534,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,10 +555,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -551,23 +567,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -820,11 +836,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L173"/>
+  <dimension ref="A1:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -875,30 +889,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -910,14 +924,14 @@
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>13</v>
@@ -938,14 +952,14 @@
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
@@ -966,19 +980,19 @@
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
         <v>12</v>
@@ -994,19 +1008,19 @@
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
         <v>12</v>
@@ -1015,21 +1029,21 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" s="25" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>13</v>
@@ -1043,76 +1057,78 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+    <row r="8" spans="1:12" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="C8" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
@@ -1125,22 +1141,22 @@
       <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1151,72 +1167,72 @@
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+        <v>48</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>13</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
@@ -1225,55 +1241,81 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="22">
+    <row r="15" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
+        <v>15</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="145" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E145" s="28"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E146" s="28"/>
+      <c r="E146" s="26"/>
     </row>
     <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E147" s="28"/>
+      <c r="E147" s="26"/>
     </row>
     <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E148" s="28"/>
-    </row>
-    <row r="170" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E170" s="28"/>
+      <c r="E148" s="26"/>
+    </row>
+    <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E149" s="26"/>
     </row>
     <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E171" s="28"/>
+      <c r="E171" s="26"/>
     </row>
     <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E172" s="28"/>
+      <c r="E172" s="26"/>
     </row>
     <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E173" s="28"/>
+      <c r="E173" s="26"/>
+    </row>
+    <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E174" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1282,31 +1324,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
-      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
-      <Description>JFHTZT72FDVU-254938863-279</Description>
-    </_dlc_DocIdUrl>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
-    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100135AEE51B13C7A4784C7A6FB658DD0E0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2ccf66da846160ccad12796df698db1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa7e5010-1311-4096-a344-326d1919664c" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="255ceb00-0504-4451-971c-89cf8ee3ad27" xmlns:ns5="953edb04-63dd-49ba-ad7b-e9d17e0e7f06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd9e9067e801230649229059a2f6238c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="fa7e5010-1311-4096-a344-326d1919664c"/>
@@ -1552,6 +1569,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
+      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
+      <Description>JFHTZT72FDVU-254938863-279</Description>
+    </_dlc_DocIdUrl>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
+    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -1603,9 +1645,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1630,22 +1685,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add JSONs for custom components, specify document support level in Excel.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d50155\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C6B73-60C3-4A92-A623-936547AB6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE92154-7403-4F32-B1E6-6AC1F891F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -838,7 +838,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -846,7 +848,7 @@
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.54296875" customWidth="1"/>
     <col min="4" max="4" width="41.453125" customWidth="1"/>
-    <col min="5" max="5" width="143.81640625" customWidth="1"/>
+    <col min="5" max="5" width="156.90625" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" customWidth="1"/>
     <col min="7" max="12" width="15" customWidth="1"/>
   </cols>
@@ -1106,7 +1108,9 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -1132,7 +1136,9 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1158,7 +1164,9 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1184,7 +1192,9 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1210,7 +1220,9 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="I13" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -1236,7 +1248,9 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1262,7 +1276,9 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1288,7 +1304,9 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>

</xml_diff>

<commit_message>
DALA-5781: Nuclear and Gas to Assembled (#1273)
---------

Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d50155\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C6B73-60C3-4A92-A623-936547AB6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE92154-7403-4F32-B1E6-6AC1F891F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -838,7 +838,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -846,7 +848,7 @@
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.54296875" customWidth="1"/>
     <col min="4" max="4" width="41.453125" customWidth="1"/>
-    <col min="5" max="5" width="143.81640625" customWidth="1"/>
+    <col min="5" max="5" width="156.90625" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" customWidth="1"/>
     <col min="7" max="12" width="15" customWidth="1"/>
   </cols>
@@ -1106,7 +1108,9 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -1132,7 +1136,9 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1158,7 +1164,9 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1184,7 +1192,9 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1210,7 +1220,9 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="I13" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -1236,7 +1248,9 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1262,7 +1276,9 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1288,7 +1304,9 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>

</xml_diff>

<commit_message>
DALA-5898: Mapping for NaG
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC24BA-2EA5-4C98-A0CA-A44DBB4D8F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B03F959-413D-44B9-80A4-61394A15666C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -188,6 +188,51 @@
   </si>
   <si>
     <t>Alias Export</t>
+  </si>
+  <si>
+    <t>REFERENCED_REPORTS</t>
+  </si>
+  <si>
+    <t>NUCLEAR_SECTION_4-26_RD</t>
+  </si>
+  <si>
+    <t>NUCLEAR_SECTION_4-27_CONSTRUCTION</t>
+  </si>
+  <si>
+    <t>NUCLEAR_SECTION_4-28_SAFE_OPERATION</t>
+  </si>
+  <si>
+    <t>FOSSIL_SECTION_4-29_CONSTRUCTION_ELECTRIC</t>
+  </si>
+  <si>
+    <t>FOSSIL_SECTION_4-30_RD_CONSTRUCTION_POWER</t>
+  </si>
+  <si>
+    <t>FOSSIL_SECTION_4-31_HEAT_GEN</t>
+  </si>
+  <si>
+    <t>REV_ALIGNED_DENOMINATOR</t>
+  </si>
+  <si>
+    <t>CAPEX_ALIGNED_DENOMINATOR</t>
+  </si>
+  <si>
+    <t>REV_ALIGNED_NUMERATOR</t>
+  </si>
+  <si>
+    <t>CAPEX_ALIGNED_NUMERATOR</t>
+  </si>
+  <si>
+    <t>REV_NON_ALIGNED_ELIGIBLE</t>
+  </si>
+  <si>
+    <t>CAPEX_NON_ALIGNED_ELIGIBLE</t>
+  </si>
+  <si>
+    <t>REV_NON_ELIGIBLE</t>
+  </si>
+  <si>
+    <t>CAPEX_NON_ELIGIBLE</t>
   </si>
 </sst>
 </file>
@@ -500,7 +545,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -588,10 +633,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -848,21 +890,21 @@
   <dimension ref="A1:M174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="5" width="41.42578125" customWidth="1"/>
-    <col min="6" max="6" width="156.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" customWidth="1"/>
+    <col min="4" max="5" width="41.453125" customWidth="1"/>
+    <col min="6" max="6" width="156.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
     <col min="8" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -916,7 +958,9 @@
       <c r="D2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
@@ -932,7 +976,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -945,7 +989,9 @@
       <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
@@ -961,7 +1007,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -974,7 +1020,9 @@
       <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
@@ -990,7 +1038,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1003,7 +1051,9 @@
       <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1019,7 +1069,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1032,7 +1082,9 @@
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1048,7 +1100,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1061,7 +1113,9 @@
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1131,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" s="11" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -1090,7 +1144,9 @@
       <c r="D8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
@@ -1106,7 +1162,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1119,7 +1175,9 @@
       <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="30"/>
+      <c r="E9" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="F9" s="13" t="s">
         <v>41</v>
       </c>
@@ -1135,7 +1193,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1148,7 +1206,9 @@
       <c r="D10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="30"/>
+      <c r="E10" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="F10" s="13" t="s">
         <v>42</v>
       </c>
@@ -1164,7 +1224,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1177,7 +1237,9 @@
       <c r="D11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="13" t="s">
         <v>40</v>
       </c>
@@ -1193,7 +1255,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1206,7 +1268,9 @@
       <c r="D12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="F12" s="13" t="s">
         <v>39</v>
       </c>
@@ -1222,7 +1286,7 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1235,7 +1299,9 @@
       <c r="D13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F13" s="16" t="s">
         <v>43</v>
       </c>
@@ -1251,7 +1317,7 @@
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -1264,7 +1330,9 @@
       <c r="D14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="F14" s="16" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1348,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -1293,7 +1361,9 @@
       <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="F15" s="13" t="s">
         <v>45</v>
       </c>
@@ -1309,7 +1379,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" s="11" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -1322,7 +1392,9 @@
       <c r="D16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="30"/>
+      <c r="E16" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="F16" s="8" t="s">
         <v>46</v>
       </c>
@@ -1338,28 +1410,28 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="146" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F146" s="26"/>
     </row>
-    <row r="147" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F147" s="26"/>
     </row>
-    <row r="148" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F148" s="26"/>
     </row>
-    <row r="149" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F149" s="26"/>
     </row>
-    <row r="171" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F171" s="26"/>
     </row>
-    <row r="172" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F172" s="26"/>
     </row>
-    <row r="173" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F173" s="26"/>
     </row>
-    <row r="174" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="6:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F174" s="26"/>
     </row>
   </sheetData>
@@ -1369,6 +1441,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1418,32 +1499,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
-      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
-      <Description>JFHTZT72FDVU-254938863-279</Description>
-    </_dlc_DocIdUrl>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
-    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100135AEE51B13C7A4784C7A6FB658DD0E0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2ccf66da846160ccad12796df698db1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa7e5010-1311-4096-a344-326d1919664c" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="255ceb00-0504-4451-971c-89cf8ee3ad27" xmlns:ns5="953edb04-63dd-49ba-ad7b-e9d17e0e7f06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd9e9067e801230649229059a2f6238c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="fa7e5010-1311-4096-a344-326d1919664c"/>
@@ -1689,7 +1745,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
+      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
+      <Description>JFHTZT72FDVU-254938863-279</Description>
+    </_dlc_DocIdUrl>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
+    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E0ED53-E837-41F7-A9C9-5E67E49390EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -1697,34 +1777,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7017BB2C-A3F1-4167-848C-B358A8DC1CB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1743,4 +1796,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7017BB2C-A3F1-4167-848C-B358A8DC1CB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DALA-5898: Field names for export (#1259)
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
+++ b/dataland-framework-toolbox/inputs/nuclear-and-gas/nuclear-and-gas.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d50155\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\nuclear-and-gas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE92154-7403-4F32-B1E6-6AC1F891F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE4FEA3-54F1-4B5F-AAB2-3A54C68D5539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -185,6 +198,54 @@
   </si>
   <si>
     <t> </t>
+  </si>
+  <si>
+    <t>Alias Export</t>
+  </si>
+  <si>
+    <t>REFERENCED_REPORTS</t>
+  </si>
+  <si>
+    <t>NUCLEAR_ENERGY_ACTIVITIES_SEC_4_26</t>
+  </si>
+  <si>
+    <t>NUCLEAR_ENERGY_ACTIVITIES_SEC_4_27</t>
+  </si>
+  <si>
+    <t>NUCLEAR_ENERGY_ACTIVITIES_SEC_4_28</t>
+  </si>
+  <si>
+    <t>FOSSIL_GAS_ACTIVITIES_SEC_4_29</t>
+  </si>
+  <si>
+    <t>FOSSIL_GAS_ACTIVITIES_SEC_4_30</t>
+  </si>
+  <si>
+    <t>FOSSIL_GAS_ACTIVITIES_SEC_4_31</t>
+  </si>
+  <si>
+    <t>REV_ALIGNED_DENOMINATOR</t>
+  </si>
+  <si>
+    <t>CAPEX_ALIGNED_DENOMINATOR</t>
+  </si>
+  <si>
+    <t>REV_ALIGNED_NUMERATOR</t>
+  </si>
+  <si>
+    <t>CAPEX_ALIGNED_NUMERATOR</t>
+  </si>
+  <si>
+    <t>REV_NON_ALIGNED</t>
+  </si>
+  <si>
+    <t>CAPEX_NON_ALIGNED</t>
+  </si>
+  <si>
+    <t>REV_NON_ELIGIBLE</t>
+  </si>
+  <si>
+    <t>CAPEX_NON_ELIGIBLE</t>
   </si>
 </sst>
 </file>
@@ -836,24 +897,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L174"/>
+  <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" customWidth="1"/>
-    <col min="5" max="5" width="156.90625" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="12" width="15" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="5" width="41.42578125" customWidth="1"/>
+    <col min="6" max="6" width="156.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,31 +928,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -905,21 +969,24 @@
         <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -933,21 +1000,24 @@
         <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -961,21 +1031,24 @@
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -989,21 +1062,24 @@
         <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1017,21 +1093,24 @@
         <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1045,21 +1124,24 @@
         <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" s="11" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -1073,21 +1155,24 @@
         <v>23</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1100,22 +1185,25 @@
       <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="G9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1128,22 +1216,25 @@
       <c r="D10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1156,22 +1247,25 @@
       <c r="D11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1184,22 +1278,25 @@
       <c r="D12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5" t="s">
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1212,22 +1309,25 @@
       <c r="D13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18" t="s">
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="18"/>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
-    </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="18"/>
+    </row>
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -1240,22 +1340,25 @@
       <c r="D14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -1268,22 +1371,25 @@
       <c r="D15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" s="11" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" s="11" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -1296,44 +1402,47 @@
       <c r="D16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
-    </row>
-    <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E146" s="26"/>
-    </row>
-    <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E147" s="26"/>
-    </row>
-    <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E148" s="26"/>
-    </row>
-    <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E149" s="26"/>
-    </row>
-    <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E171" s="26"/>
-    </row>
-    <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E172" s="26"/>
-    </row>
-    <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E173" s="26"/>
-    </row>
-    <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E174" s="26"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="146" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F146" s="26"/>
+    </row>
+    <row r="147" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F147" s="26"/>
+    </row>
+    <row r="148" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F148" s="26"/>
+    </row>
+    <row r="149" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F149" s="26"/>
+    </row>
+    <row r="171" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F171" s="26"/>
+    </row>
+    <row r="172" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F172" s="26"/>
+    </row>
+    <row r="173" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F173" s="26"/>
+    </row>
+    <row r="174" spans="6:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F174" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>